<commit_message>
Changed Naval Pilots locations
</commit_message>
<xml_diff>
--- a/WITPAE Pilots Create.xlsx
+++ b/WITPAE Pilots Create.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Other\WITPAE\WITPGIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Other\WITPAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot" sheetId="4" r:id="rId1"/>
@@ -695,9 +695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,7 +1990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Z7" sqref="Z7"/>
     </sheetView>

</xml_diff>

<commit_message>
Added DaBabes JJ Dec 7
</commit_message>
<xml_diff>
--- a/WITPAE Pilots Create.xlsx
+++ b/WITPAE Pilots Create.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="90">
   <si>
     <t>USMC</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Burkes, S.</t>
-  </si>
-  <si>
-    <t>CAPT</t>
   </si>
   <si>
     <t>Hima, M.</t>
@@ -688,9 +685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,33 +703,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1">
         <v>1694</v>
@@ -741,10 +738,10 @@
         <v>7000</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="5">
         <v>85</v>
@@ -753,22 +750,22 @@
         <v>24022</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3">
         <v>7001</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="5">
         <v>80</v>
@@ -777,22 +774,22 @@
         <v>24001</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
         <v>7002</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="5">
         <v>75</v>
@@ -801,46 +798,46 @@
         <v>24006</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
         <v>7003</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="5">
         <v>65</v>
       </c>
       <c r="G5" s="5">
-        <v>24022</v>
+        <v>24000</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
         <v>7004</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="5">
         <v>70</v>
@@ -849,54 +846,54 @@
         <v>24005</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
         <v>7005</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="5">
         <v>70</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
         <v>7006</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="5">
         <v>65</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1">
         <v>1712</v>
@@ -905,10 +902,10 @@
         <v>7010</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="5">
         <v>70</v>
@@ -917,22 +914,22 @@
         <v>24002</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11">
         <v>7011</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="5">
         <v>75</v>
@@ -941,22 +938,22 @@
         <v>24007</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12">
         <v>7012</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="5">
         <v>75</v>
@@ -965,96 +962,96 @@
         <v>24015</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13">
         <v>7013</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="5">
         <v>65</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14">
         <v>7014</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="5">
         <v>65</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15">
         <v>7015</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="5">
         <v>65</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16">
         <v>7016</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="5">
         <v>65</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1">
         <v>1700</v>
@@ -1063,10 +1060,10 @@
         <v>7020</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="5">
         <v>75</v>
@@ -1075,22 +1072,22 @@
         <v>24014</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19">
         <v>7021</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="5">
         <v>65</v>
@@ -1099,117 +1096,117 @@
         <v>24009</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20">
         <v>7022</v>
       </c>
       <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F20" s="5">
         <v>70</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21">
         <v>7023</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="5">
         <v>65</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22">
         <v>7024</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" s="5">
         <v>65</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23">
         <v>7025</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="5">
         <v>65</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24">
         <v>7026</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="5">
         <v>70</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="1">
         <v>1706</v>
@@ -1218,10 +1215,10 @@
         <v>7030</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F26" s="5">
         <v>70</v>
@@ -1230,22 +1227,22 @@
         <v>24003</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27">
         <v>7031</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F27" s="5">
         <v>65</v>
@@ -1254,22 +1251,22 @@
         <v>24008</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28">
         <v>7032</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" s="5">
         <v>75</v>
@@ -1278,75 +1275,75 @@
         <v>24011</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29">
         <v>7033</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" s="5">
         <v>65</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30">
         <v>7034</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="5">
         <v>65</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31">
         <v>7035</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" s="5">
         <v>65</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1">
         <v>2603</v>
@@ -1355,10 +1352,10 @@
         <v>7040</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F33" s="5">
         <v>72</v>
@@ -1372,17 +1369,17 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34">
         <v>7041</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F34" s="5">
         <v>65</v>
@@ -1396,17 +1393,17 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35">
         <v>7042</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" s="5">
         <v>75</v>
@@ -1420,17 +1417,17 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36">
         <v>7043</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F36" s="5">
         <v>75</v>
@@ -1441,14 +1438,14 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37">
         <v>7044</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>1</v>
@@ -1462,7 +1459,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>7045</v>
@@ -1482,7 +1479,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1">
         <v>2588</v>
@@ -1491,10 +1488,10 @@
         <v>7050</v>
       </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F40" s="5">
         <v>80</v>
@@ -1508,17 +1505,17 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41">
         <v>7051</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F41" s="5">
         <v>70</v>
@@ -1532,17 +1529,17 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42">
         <v>7052</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" s="5">
         <v>70</v>
@@ -1556,14 +1553,14 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43">
         <v>7053</v>
       </c>
       <c r="D43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>1</v>
@@ -1577,14 +1574,14 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44">
         <v>7054</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>1</v>
@@ -1598,14 +1595,14 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45">
         <v>7055</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>1</v>
@@ -1619,7 +1616,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" s="1">
         <v>1723</v>
@@ -1628,60 +1625,60 @@
         <v>7060</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48">
         <v>7061</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49">
         <v>7062</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50">
         <v>7063</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51">
         <v>7064</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="1">
         <v>2561</v>
@@ -1690,10 +1687,10 @@
         <v>7070</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F53" s="5">
         <v>75</v>
@@ -1707,17 +1704,17 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54">
         <v>7071</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F54" s="5">
         <v>80</v>
@@ -1731,17 +1728,17 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55">
         <v>7072</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" s="5">
         <v>65</v>
@@ -1752,17 +1749,17 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56">
         <v>7073</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" s="5">
         <v>70</v>
@@ -1773,14 +1770,14 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57">
         <v>7074</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>1</v>
@@ -1794,13 +1791,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58">
         <v>7075</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>1</v>
@@ -1814,7 +1811,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B60" s="1">
         <v>2553</v>
@@ -1823,10 +1820,10 @@
         <v>7080</v>
       </c>
       <c r="D60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F60" s="5">
         <v>75</v>
@@ -1840,17 +1837,17 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61">
         <v>7081</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F61" s="5">
         <v>75</v>
@@ -1864,17 +1861,17 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62">
         <v>7082</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F62" s="5">
         <v>70</v>
@@ -1888,17 +1885,17 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63">
         <v>7083</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" s="5">
         <v>70</v>
@@ -1912,17 +1909,17 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64">
         <v>7084</v>
       </c>
       <c r="D64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" s="5">
         <v>75</v>
@@ -1933,13 +1930,13 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C65">
         <v>7085</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>1</v>
@@ -1953,13 +1950,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C66">
         <v>7086</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>1</v>
@@ -1973,7 +1970,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73" s="1">
         <v>2589</v>
@@ -1987,7 +1984,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74">
@@ -1999,7 +1996,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75">
@@ -2011,7 +2008,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76">
@@ -2023,7 +2020,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77">
@@ -2043,9 +2040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,7 +2079,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="3">
         <v>23999</v>
@@ -2168,212 +2165,212 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Z2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>0</v>
@@ -2382,10 +2379,10 @@
         <v>0</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>0</v>
@@ -2406,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>0</v>
@@ -2417,7 +2414,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3">
         <v>85</v>
@@ -2500,7 +2497,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3">
         <v>90</v>
@@ -2583,7 +2580,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3">
         <v>90</v>
@@ -2637,7 +2634,7 @@
         <v>50</v>
       </c>
       <c r="S7" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="T7" s="2">
         <v>50</v>
@@ -2646,7 +2643,7 @@
         <v>50</v>
       </c>
       <c r="V7" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="W7" s="2">
         <v>50</v>
@@ -2666,7 +2663,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3">
         <v>90</v>
@@ -2749,7 +2746,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3">
         <v>75</v>
@@ -2832,7 +2829,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3">
         <v>95</v>
@@ -2915,7 +2912,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3">
         <v>80</v>
@@ -2945,7 +2942,7 @@
         <v>70</v>
       </c>
       <c r="K11" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L11" s="2">
         <v>70</v>
@@ -2960,37 +2957,37 @@
         <v>65</v>
       </c>
       <c r="P11" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q11" s="2">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="R11" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S11" s="2">
         <v>70</v>
       </c>
       <c r="T11" s="2">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="U11" s="2">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="V11" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="W11" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="X11" s="2">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="Y11" s="2">
         <v>75</v>
       </c>
       <c r="Z11" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AA11" s="2">
         <v>75</v>
@@ -2998,7 +2995,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
Added stock scen 1 scenario.
</commit_message>
<xml_diff>
--- a/WITPAE Pilots Create.xlsx
+++ b/WITPAE Pilots Create.xlsx
@@ -686,8 +686,8 @@
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,11 +2038,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O3" sqref="O3"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,22 +2453,22 @@
         <v>75</v>
       </c>
       <c r="N5" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="O5" s="2">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="P5" s="2">
         <v>70</v>
       </c>
       <c r="Q5" s="2">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="R5" s="2">
         <v>75</v>
       </c>
       <c r="S5" s="2">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="T5" s="2">
         <v>70</v>
@@ -2533,10 +2533,10 @@
         <v>75</v>
       </c>
       <c r="M6" s="2">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="N6" s="2">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="O6" s="2">
         <v>75</v>
@@ -2545,13 +2545,13 @@
         <v>75</v>
       </c>
       <c r="Q6" s="2">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="R6" s="2">
         <v>75</v>
       </c>
       <c r="S6" s="2">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="T6" s="2">
         <v>75</v>
@@ -2569,7 +2569,7 @@
         <v>75</v>
       </c>
       <c r="Y6" s="2">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="Z6" s="2">
         <v>75</v>
@@ -2619,7 +2619,7 @@
         <v>50</v>
       </c>
       <c r="N7" s="2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="O7" s="2">
         <v>50</v>
@@ -2634,7 +2634,7 @@
         <v>50</v>
       </c>
       <c r="S7" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="T7" s="2">
         <v>50</v>
@@ -2643,7 +2643,7 @@
         <v>50</v>
       </c>
       <c r="V7" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="W7" s="2">
         <v>50</v>
@@ -2652,7 +2652,7 @@
         <v>50</v>
       </c>
       <c r="Y7" s="2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="Z7" s="2">
         <v>50</v>
@@ -2699,25 +2699,25 @@
         <v>70</v>
       </c>
       <c r="M8" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="N8" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="O8" s="2">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="P8" s="2">
         <v>70</v>
       </c>
       <c r="Q8" s="2">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="R8" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="S8" s="2">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="T8" s="2">
         <v>70</v>
@@ -2735,13 +2735,13 @@
         <v>70</v>
       </c>
       <c r="Y8" s="2">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Z8" s="2">
         <v>70</v>
       </c>
       <c r="AA8" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -2764,7 +2764,7 @@
         <v>80</v>
       </c>
       <c r="G9" s="2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2">
         <v>60</v>
@@ -2782,10 +2782,10 @@
         <v>60</v>
       </c>
       <c r="M9" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="N9" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O9" s="2">
         <v>60</v>
@@ -2794,13 +2794,13 @@
         <v>70</v>
       </c>
       <c r="Q9" s="2">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="R9" s="2">
         <v>60</v>
       </c>
       <c r="S9" s="2">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="T9" s="2">
         <v>70</v>
@@ -2818,13 +2818,13 @@
         <v>70</v>
       </c>
       <c r="Y9" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>70</v>
+      </c>
+      <c r="AA9" s="2">
         <v>60</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>70</v>
-      </c>
-      <c r="AA9" s="2">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -2844,10 +2844,10 @@
         <v>70</v>
       </c>
       <c r="F10" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G10" s="2">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H10" s="2">
         <v>85</v>
@@ -2865,22 +2865,22 @@
         <v>85</v>
       </c>
       <c r="M10" s="2">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="N10" s="2">
+        <v>75</v>
+      </c>
+      <c r="O10" s="2">
         <v>85</v>
       </c>
-      <c r="O10" s="2">
-        <v>80</v>
-      </c>
       <c r="P10" s="2">
         <v>75</v>
       </c>
       <c r="Q10" s="2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="R10" s="2">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="S10" s="2">
         <v>90</v>
@@ -2901,13 +2901,13 @@
         <v>75</v>
       </c>
       <c r="Y10" s="2">
+        <v>90</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA10" s="2">
         <v>85</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -2930,40 +2930,40 @@
         <v>70</v>
       </c>
       <c r="G11" s="2">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H11" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I11" s="2">
         <v>65</v>
       </c>
       <c r="J11" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K11" s="2">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="L11" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="M11" s="2">
         <v>65</v>
       </c>
       <c r="N11" s="2">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="O11" s="2">
         <v>65</v>
       </c>
       <c r="P11" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q11" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R11" s="2">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="S11" s="2">
         <v>70</v>
@@ -2975,22 +2975,22 @@
         <v>65</v>
       </c>
       <c r="V11" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="W11" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="X11" s="2">
         <v>65</v>
       </c>
       <c r="Y11" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Z11" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AA11" s="2">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -3074,6 +3074,74 @@
       </c>
       <c r="AA12" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>2</v>
+      </c>
+      <c r="M14" s="2">
+        <v>2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2">
+        <v>2</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>3</v>
+      </c>
+      <c r="R14" s="2">
+        <v>2</v>
+      </c>
+      <c r="S14" s="2">
+        <v>3</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1</v>
+      </c>
+      <c r="V14" s="2">
+        <v>1</v>
+      </c>
+      <c r="W14" s="2">
+        <v>1</v>
+      </c>
+      <c r="X14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Stock Dec 8 Scen
</commit_message>
<xml_diff>
--- a/WITPAE Pilots Create.xlsx
+++ b/WITPAE Pilots Create.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Other\WITPAE\WITPGIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\WITPAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{129C2824-3F22-4669-8880-94E285061A00}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot" sheetId="4" r:id="rId1"/>
     <sheet name="Leader" sheetId="5" r:id="rId2"/>
+    <sheet name="TrainingSquadrons" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="121">
   <si>
     <t>USMC</t>
   </si>
@@ -290,12 +292,105 @@
   </si>
   <si>
     <t>Mathews, C.</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Formation</t>
+  </si>
+  <si>
+    <t>Aircraft</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>Duffield, C.</t>
+  </si>
+  <si>
+    <t>Harvey, J.</t>
+  </si>
+  <si>
+    <t>VFT-1001</t>
+  </si>
+  <si>
+    <t>VFT-1002</t>
+  </si>
+  <si>
+    <t>VBT-1003</t>
+  </si>
+  <si>
+    <t>VBT-1004</t>
+  </si>
+  <si>
+    <t>VTT-1005</t>
+  </si>
+  <si>
+    <t>VTT-1006</t>
+  </si>
+  <si>
+    <t>VOT-1007</t>
+  </si>
+  <si>
+    <t>VOT-1008</t>
+  </si>
+  <si>
+    <t>VPT-1009</t>
+  </si>
+  <si>
+    <t>VPT-1010</t>
+  </si>
+  <si>
+    <t>VRT-1011</t>
+  </si>
+  <si>
+    <t>VMFT-2001</t>
+  </si>
+  <si>
+    <t>VMFT-2002</t>
+  </si>
+  <si>
+    <t>VMSBT-2003</t>
+  </si>
+  <si>
+    <t>VMSBT-2004</t>
+  </si>
+  <si>
+    <t>VMJT-2005</t>
+  </si>
+  <si>
+    <t>VMDT-2006</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>TFS-3001</t>
+  </si>
+  <si>
+    <t>TFS-3002</t>
+  </si>
+  <si>
+    <t>TBS-3003</t>
+  </si>
+  <si>
+    <t>TBS-3004</t>
+  </si>
+  <si>
+    <t>TOS-3005</t>
+  </si>
+  <si>
+    <t>TTS-3006</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -682,12 +777,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +863,7 @@
         <v>71</v>
       </c>
       <c r="F3" s="5">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G3" s="5">
         <v>24001</v>
@@ -1307,14 +1402,14 @@
       <c r="C30">
         <v>7034</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>38</v>
+      <c r="D30" t="s">
+        <v>94</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F30" s="5">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>10</v>
@@ -1328,8 +1423,8 @@
       <c r="C31">
         <v>7035</v>
       </c>
-      <c r="D31" t="s">
-        <v>28</v>
+      <c r="D31" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>11</v>
@@ -1341,51 +1436,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2603</v>
-      </c>
-      <c r="C33">
-        <v>7040</v>
-      </c>
-      <c r="D33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="5">
-        <v>72</v>
-      </c>
-      <c r="G33" s="5">
-        <v>24004</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>0</v>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32">
+        <v>7035</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="5">
+        <v>65</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1">
+        <v>2603</v>
+      </c>
       <c r="C34">
-        <v>7041</v>
+        <v>7040</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F34" s="5">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="G34" s="5">
-        <v>24012</v>
+        <v>24004</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>0</v>
@@ -1397,19 +1489,19 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35">
-        <v>7042</v>
+        <v>7041</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F35" s="5">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G35" s="5">
-        <v>24023</v>
+        <v>24012</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>0</v>
@@ -1421,10 +1513,10 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36">
-        <v>7043</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>87</v>
+        <v>7042</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>4</v>
@@ -1432,6 +1524,9 @@
       <c r="F36" s="5">
         <v>75</v>
       </c>
+      <c r="G36" s="5">
+        <v>24023</v>
+      </c>
       <c r="H36" s="5" t="s">
         <v>0</v>
       </c>
@@ -1442,16 +1537,16 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37">
-        <v>7044</v>
-      </c>
-      <c r="D37" t="s">
-        <v>23</v>
+        <v>7043</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F37" s="5">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>0</v>
@@ -1461,11 +1556,12 @@
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="B38" s="1"/>
       <c r="C38">
-        <v>7045</v>
+        <v>7044</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>1</v>
@@ -1477,29 +1573,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="1">
-        <v>2588</v>
-      </c>
-      <c r="C40">
-        <v>7050</v>
-      </c>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F40" s="5">
-        <v>80</v>
-      </c>
-      <c r="G40" s="5">
-        <v>24016</v>
-      </c>
-      <c r="H40" s="5" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39">
+        <v>7045</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="5">
+        <v>65</v>
+      </c>
+      <c r="H39" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1507,21 +1597,23 @@
       <c r="A41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="1">
+        <v>2588</v>
+      </c>
       <c r="C41">
-        <v>7051</v>
+        <v>7050</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F41" s="5">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G41" s="5">
-        <v>24017</v>
+        <v>24016</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>0</v>
@@ -1533,19 +1625,19 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42">
-        <v>7052</v>
+        <v>7051</v>
       </c>
       <c r="D42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F42" s="5">
         <v>70</v>
       </c>
       <c r="G42" s="5">
-        <v>24013</v>
+        <v>24017</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>0</v>
@@ -1557,16 +1649,19 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43">
-        <v>7053</v>
+        <v>7052</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F43" s="5">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="G43" s="5">
+        <v>24013</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>0</v>
@@ -1578,13 +1673,13 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44">
-        <v>7054</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>19</v>
+        <v>7053</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F44" s="5">
         <v>65</v>
@@ -1599,10 +1694,10 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45">
-        <v>7055</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>89</v>
+        <v>7054</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>1</v>
@@ -1614,39 +1709,57 @@
         <v>0</v>
       </c>
     </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46">
+        <v>7055</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5">
+        <v>65</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="1">
-        <v>1723</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B47" s="1"/>
       <c r="C47">
-        <v>7060</v>
+        <v>7056</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="5">
+        <v>65</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="1"/>
-      <c r="C48">
-        <v>7061</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1">
+        <v>1723</v>
+      </c>
       <c r="C49">
-        <v>7062</v>
+        <v>7060</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>10</v>
@@ -1658,7 +1771,7 @@
       </c>
       <c r="B50" s="1"/>
       <c r="C50">
-        <v>7063</v>
+        <v>7061</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>10</v>
@@ -1670,78 +1783,57 @@
       </c>
       <c r="B51" s="1"/>
       <c r="C51">
-        <v>7064</v>
+        <v>7062</v>
       </c>
       <c r="H51" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52">
+        <v>7063</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" s="1">
-        <v>2561</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B53" s="1"/>
       <c r="C53">
-        <v>7070</v>
-      </c>
-      <c r="D53" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F53" s="5">
-        <v>75</v>
-      </c>
-      <c r="G53" s="5">
-        <v>24018</v>
+        <v>7064</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="1"/>
-      <c r="C54">
-        <v>7071</v>
-      </c>
-      <c r="D54" t="s">
-        <v>81</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F54" s="5">
-        <v>80</v>
-      </c>
-      <c r="G54" s="5">
-        <v>24024</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="1"/>
+      <c r="B55" s="1">
+        <v>2561</v>
+      </c>
       <c r="C55">
-        <v>7072</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>57</v>
+        <v>7070</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F55" s="5">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="G55" s="5">
+        <v>24018</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>0</v>
@@ -1753,16 +1845,19 @@
       </c>
       <c r="B56" s="1"/>
       <c r="C56">
-        <v>7073</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>88</v>
+        <v>7071</v>
+      </c>
+      <c r="D56" t="s">
+        <v>81</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F56" s="5">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c r="G56" s="5">
+        <v>24024</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>0</v>
@@ -1774,13 +1869,13 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57">
-        <v>7074</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>80</v>
+        <v>7072</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F57" s="5">
         <v>65</v>
@@ -1793,69 +1888,61 @@
       <c r="A58" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="B58" s="1"/>
       <c r="C58">
-        <v>7075</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>82</v>
+        <v>7073</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E58" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="5">
+        <v>70</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59">
+        <v>7074</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F58" s="5">
-        <v>65</v>
-      </c>
-      <c r="H58" s="5" t="s">
+      <c r="F59" s="5">
+        <v>65</v>
+      </c>
+      <c r="H59" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="1">
-        <v>2553</v>
+        <v>67</v>
       </c>
       <c r="C60">
-        <v>7080</v>
-      </c>
-      <c r="D60" t="s">
-        <v>3</v>
+        <v>7075</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="F60" s="5">
-        <v>75</v>
-      </c>
-      <c r="G60" s="5">
-        <v>24020</v>
+        <v>65</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="C61">
-        <v>7081</v>
-      </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F61" s="5">
-        <v>75</v>
-      </c>
-      <c r="G61" s="5">
-        <v>24019</v>
-      </c>
-      <c r="H61" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1863,21 +1950,23 @@
       <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="1"/>
+      <c r="B62" s="1">
+        <v>2553</v>
+      </c>
       <c r="C62">
-        <v>7082</v>
+        <v>7080</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F62" s="5">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G62" s="5">
-        <v>24021</v>
+        <v>24020</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>0</v>
@@ -1889,19 +1978,19 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63">
-        <v>7083</v>
+        <v>7081</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F63" s="5">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G63" s="5">
-        <v>24010</v>
+        <v>24019</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>0</v>
@@ -1913,16 +2002,19 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64">
-        <v>7084</v>
+        <v>7082</v>
       </c>
       <c r="D64" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F64" s="5">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="G64" s="5">
+        <v>24021</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>0</v>
@@ -1932,17 +2024,21 @@
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="B65" s="1"/>
       <c r="C65">
-        <v>7085</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>86</v>
+        <v>7083</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F65" s="5">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="G65" s="5">
+        <v>24010</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>0</v>
@@ -1952,19 +2048,98 @@
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="B66" s="1"/>
       <c r="C66">
+        <v>7084</v>
+      </c>
+      <c r="D66" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="5">
+        <v>75</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67">
+        <v>7085</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="5">
+        <v>65</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C68">
         <v>7086</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D68" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F66" s="5">
-        <v>65</v>
-      </c>
-      <c r="H66" s="5" t="s">
+      <c r="F68" s="5">
+        <v>65</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2589</v>
+      </c>
+      <c r="C70">
+        <v>7090</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71">
+        <v>7091</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72">
+        <v>7092</v>
+      </c>
+      <c r="H72" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1972,11 +2147,9 @@
       <c r="A73" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="1">
-        <v>2589</v>
-      </c>
+      <c r="B73" s="1"/>
       <c r="C73">
-        <v>7090</v>
+        <v>7093</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>0</v>
@@ -1988,45 +2161,9 @@
       </c>
       <c r="B74" s="1"/>
       <c r="C74">
-        <v>7091</v>
+        <v>7094</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B75" s="1"/>
-      <c r="C75">
-        <v>7092</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="1"/>
-      <c r="C76">
-        <v>7093</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" s="1"/>
-      <c r="C77">
-        <v>7094</v>
-      </c>
-      <c r="H77" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2037,15 +2174,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -2868,7 +3005,7 @@
         <v>85</v>
       </c>
       <c r="N10" s="2">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="O10" s="2">
         <v>85</v>
@@ -2960,7 +3097,7 @@
         <v>65</v>
       </c>
       <c r="Q11" s="2">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="R11" s="2">
         <v>65</v>
@@ -2998,82 +3135,82 @@
         <v>49</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -3142,6 +3279,499 @@
       </c>
       <c r="AA14" s="2">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C33C302-DA62-45E2-AD4A-FE437348ABC5}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>5000</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="3">
+        <v>519</v>
+      </c>
+      <c r="E2" s="3">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>5001</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="3">
+        <v>519</v>
+      </c>
+      <c r="E3" s="3">
+        <v>24</v>
+      </c>
+      <c r="G3" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>5002</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="3">
+        <v>519</v>
+      </c>
+      <c r="E4" s="3">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>5003</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="3">
+        <v>519</v>
+      </c>
+      <c r="E5" s="3">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5004</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3">
+        <v>615</v>
+      </c>
+      <c r="E6" s="3">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5005</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="3">
+        <v>615</v>
+      </c>
+      <c r="E7" s="3">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5006</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="3">
+        <v>615</v>
+      </c>
+      <c r="E8" s="3">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>5007</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="3">
+        <v>615</v>
+      </c>
+      <c r="E9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>5008</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="3">
+        <v>615</v>
+      </c>
+      <c r="E10" s="3">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>5009</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3">
+        <v>615</v>
+      </c>
+      <c r="E11" s="3">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>5010</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="3">
+        <v>615</v>
+      </c>
+      <c r="E12" s="3">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>5020</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="3">
+        <v>506</v>
+      </c>
+      <c r="E14" s="3">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>5021</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="3">
+        <v>506</v>
+      </c>
+      <c r="E15" s="3">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>5022</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="3">
+        <v>506</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="G16" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>5023</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="3">
+        <v>506</v>
+      </c>
+      <c r="E17" s="3">
+        <v>18</v>
+      </c>
+      <c r="G17" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>5024</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="3">
+        <v>506</v>
+      </c>
+      <c r="E18" s="3">
+        <v>15</v>
+      </c>
+      <c r="G18" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>5025</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="3">
+        <v>506</v>
+      </c>
+      <c r="E19" s="3">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>5030</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="3">
+        <v>25</v>
+      </c>
+      <c r="G21" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>5031</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="3">
+        <v>25</v>
+      </c>
+      <c r="G22" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>5032</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="3">
+        <v>526</v>
+      </c>
+      <c r="E23" s="3">
+        <v>15</v>
+      </c>
+      <c r="G23" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>5033</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="3">
+        <v>526</v>
+      </c>
+      <c r="E24" s="3">
+        <v>15</v>
+      </c>
+      <c r="G24" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>5034</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="3">
+        <v>15</v>
+      </c>
+      <c r="G25" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>5035</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="3">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>